<commit_message>
ItemList.xlsx: Fixed missing values in the template file Items.data: Fixed missing values in the item list
Signed-off-by: Dasaan <mrloquax@googlemail.com>
</commit_message>
<xml_diff>
--- a/ItemList.xlsx
+++ b/ItemList.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ItemList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6406" uniqueCount="3195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6712" uniqueCount="3195">
   <si>
     <t>Aegis: Reflection</t>
   </si>
@@ -10422,7 +10422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2057" workbookViewId="0">
+      <selection activeCell="C2081" sqref="C2081"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -38532,6 +38534,9 @@
       <c r="B2555" t="s">
         <v>2397</v>
       </c>
+      <c r="C2555" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2556" spans="1:3">
       <c r="A2556">
@@ -38540,6 +38545,9 @@
       <c r="B2556" t="s">
         <v>2398</v>
       </c>
+      <c r="C2556" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2557" spans="1:3">
       <c r="A2557">
@@ -38548,6 +38556,9 @@
       <c r="B2557" t="s">
         <v>2399</v>
       </c>
+      <c r="C2557" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2558" spans="1:3">
       <c r="A2558">
@@ -38556,6 +38567,9 @@
       <c r="B2558" t="s">
         <v>2400</v>
       </c>
+      <c r="C2558" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2559" spans="1:3">
       <c r="A2559">
@@ -38564,6 +38578,9 @@
       <c r="B2559" t="s">
         <v>2401</v>
       </c>
+      <c r="C2559" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2560" spans="1:3">
       <c r="A2560">
@@ -38572,2309 +38589,3176 @@
       <c r="B2560" t="s">
         <v>2402</v>
       </c>
-    </row>
-    <row r="2561" spans="1:2">
+      <c r="C2560" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:3">
       <c r="A2561">
         <v>43342</v>
       </c>
       <c r="B2561" t="s">
         <v>2403</v>
       </c>
-    </row>
-    <row r="2562" spans="1:2">
+      <c r="C2561" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:3">
       <c r="A2562">
         <v>43343</v>
       </c>
       <c r="B2562" t="s">
         <v>2404</v>
       </c>
-    </row>
-    <row r="2563" spans="1:2">
+      <c r="C2562" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:3">
       <c r="A2563">
         <v>43344</v>
       </c>
       <c r="B2563" t="s">
         <v>2405</v>
       </c>
-    </row>
-    <row r="2564" spans="1:2">
+      <c r="C2563" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:3">
       <c r="A2564">
         <v>543197</v>
       </c>
       <c r="B2564" t="s">
         <v>2406</v>
       </c>
-    </row>
-    <row r="2565" spans="1:2">
+      <c r="C2564" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:3">
       <c r="A2565">
         <v>43341</v>
       </c>
       <c r="B2565" t="s">
         <v>2407</v>
       </c>
-    </row>
-    <row r="2566" spans="1:2">
+      <c r="C2565" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:3">
       <c r="A2566">
         <v>543198</v>
       </c>
       <c r="B2566" t="s">
         <v>2408</v>
       </c>
-    </row>
-    <row r="2567" spans="1:2">
+      <c r="C2566" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:3">
       <c r="A2567">
         <v>543199</v>
       </c>
       <c r="B2567" t="s">
         <v>2409</v>
       </c>
-    </row>
-    <row r="2568" spans="1:2">
+      <c r="C2567" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:3">
       <c r="A2568">
         <v>543200</v>
       </c>
       <c r="B2568" t="s">
         <v>2410</v>
       </c>
-    </row>
-    <row r="2569" spans="1:2">
+      <c r="C2568" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:3">
       <c r="A2569">
         <v>543201</v>
       </c>
       <c r="B2569" t="s">
         <v>2411</v>
       </c>
-    </row>
-    <row r="2570" spans="1:2">
+      <c r="C2569" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:3">
       <c r="A2570">
         <v>543202</v>
       </c>
       <c r="B2570" t="s">
         <v>2412</v>
       </c>
-    </row>
-    <row r="2571" spans="1:2">
+      <c r="C2570" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:3">
       <c r="A2571">
         <v>543203</v>
       </c>
       <c r="B2571" t="s">
         <v>2413</v>
       </c>
-    </row>
-    <row r="2572" spans="1:2">
+      <c r="C2571" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:3">
       <c r="A2572">
         <v>543204</v>
       </c>
       <c r="B2572" t="s">
         <v>2414</v>
       </c>
-    </row>
-    <row r="2573" spans="1:2">
+      <c r="C2572" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:3">
       <c r="A2573">
         <v>543205</v>
       </c>
       <c r="B2573" t="s">
         <v>2415</v>
       </c>
-    </row>
-    <row r="2574" spans="1:2">
+      <c r="C2573" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:3">
       <c r="A2574">
         <v>543206</v>
       </c>
       <c r="B2574" t="s">
         <v>2416</v>
       </c>
-    </row>
-    <row r="2575" spans="1:2">
+      <c r="C2574" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:3">
       <c r="A2575">
         <v>543207</v>
       </c>
       <c r="B2575" t="s">
         <v>2417</v>
       </c>
-    </row>
-    <row r="2576" spans="1:2">
+      <c r="C2575" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:3">
       <c r="A2576">
         <v>543208</v>
       </c>
       <c r="B2576" t="s">
         <v>2418</v>
       </c>
-    </row>
-    <row r="2577" spans="1:2">
+      <c r="C2576" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:3">
       <c r="A2577">
         <v>543209</v>
       </c>
       <c r="B2577" t="s">
         <v>2419</v>
       </c>
-    </row>
-    <row r="2578" spans="1:2">
+      <c r="C2577" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:3">
       <c r="A2578">
         <v>543210</v>
       </c>
       <c r="B2578" t="s">
         <v>2420</v>
       </c>
-    </row>
-    <row r="2579" spans="1:2">
+      <c r="C2578" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:3">
       <c r="A2579">
         <v>543213</v>
       </c>
       <c r="B2579" t="s">
         <v>2421</v>
       </c>
-    </row>
-    <row r="2580" spans="1:2">
+      <c r="C2579" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:3">
       <c r="A2580">
         <v>543212</v>
       </c>
       <c r="B2580" t="s">
         <v>2422</v>
       </c>
-    </row>
-    <row r="2581" spans="1:2">
+      <c r="C2580" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:3">
       <c r="A2581">
         <v>543211</v>
       </c>
       <c r="B2581" t="s">
         <v>2423</v>
       </c>
-    </row>
-    <row r="2582" spans="1:2">
+      <c r="C2581" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:3">
       <c r="A2582">
         <v>543214</v>
       </c>
       <c r="B2582" t="s">
         <v>2424</v>
       </c>
-    </row>
-    <row r="2583" spans="1:2">
+      <c r="C2582" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:3">
       <c r="A2583">
         <v>543215</v>
       </c>
       <c r="B2583" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="2584" spans="1:2">
+      <c r="C2583" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:3">
       <c r="A2584">
         <v>543216</v>
       </c>
       <c r="B2584" t="s">
         <v>2426</v>
       </c>
-    </row>
-    <row r="2585" spans="1:2">
+      <c r="C2584" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:3">
       <c r="A2585">
         <v>543217</v>
       </c>
       <c r="B2585" t="s">
         <v>2427</v>
       </c>
-    </row>
-    <row r="2586" spans="1:2">
+      <c r="C2585" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:3">
       <c r="A2586">
         <v>543218</v>
       </c>
       <c r="B2586" t="s">
         <v>2428</v>
       </c>
-    </row>
-    <row r="2587" spans="1:2">
+      <c r="C2586" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:3">
       <c r="A2587">
         <v>543189</v>
       </c>
       <c r="B2587" t="s">
         <v>2429</v>
       </c>
-    </row>
-    <row r="2588" spans="1:2">
+      <c r="C2587" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:3">
       <c r="A2588">
         <v>543190</v>
       </c>
       <c r="B2588" t="s">
         <v>2430</v>
       </c>
-    </row>
-    <row r="2589" spans="1:2">
+      <c r="C2588" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:3">
       <c r="A2589">
         <v>543191</v>
       </c>
       <c r="B2589" t="s">
         <v>2431</v>
       </c>
-    </row>
-    <row r="2590" spans="1:2">
+      <c r="C2589" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:3">
       <c r="A2590">
         <v>563487</v>
       </c>
       <c r="B2590" t="s">
         <v>2432</v>
       </c>
-    </row>
-    <row r="2591" spans="1:2">
+      <c r="C2590" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:3">
       <c r="A2591">
         <v>543471</v>
       </c>
       <c r="B2591" t="s">
         <v>2433</v>
       </c>
-    </row>
-    <row r="2592" spans="1:2">
+      <c r="C2591" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:3">
       <c r="A2592">
         <v>827679</v>
       </c>
       <c r="B2592" t="s">
         <v>2434</v>
       </c>
-    </row>
-    <row r="2593" spans="1:2">
+      <c r="C2592" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:3">
       <c r="A2593">
         <v>568744</v>
       </c>
       <c r="B2593" t="s">
         <v>2435</v>
       </c>
-    </row>
-    <row r="2594" spans="1:2">
+      <c r="C2593" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:3">
       <c r="A2594">
         <v>568746</v>
       </c>
       <c r="B2594" t="s">
         <v>2436</v>
       </c>
-    </row>
-    <row r="2595" spans="1:2">
+      <c r="C2594" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:3">
       <c r="A2595">
         <v>568747</v>
       </c>
       <c r="B2595" t="s">
         <v>2437</v>
       </c>
-    </row>
-    <row r="2596" spans="1:2">
+      <c r="C2595" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:3">
       <c r="A2596">
         <v>559342</v>
       </c>
       <c r="B2596" t="s">
         <v>2438</v>
       </c>
-    </row>
-    <row r="2597" spans="1:2">
+      <c r="C2596" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:3">
       <c r="A2597">
         <v>559289</v>
       </c>
       <c r="B2597" t="s">
         <v>2439</v>
       </c>
-    </row>
-    <row r="2598" spans="1:2">
+      <c r="C2597" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:3">
       <c r="A2598">
         <v>86201</v>
       </c>
       <c r="B2598" t="s">
         <v>2440</v>
       </c>
-    </row>
-    <row r="2599" spans="1:2">
+      <c r="C2598" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:3">
       <c r="A2599">
         <v>543473</v>
       </c>
       <c r="B2599" t="s">
         <v>2441</v>
       </c>
-    </row>
-    <row r="2600" spans="1:2">
+      <c r="C2599" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:3">
       <c r="A2600">
         <v>559296</v>
       </c>
       <c r="B2600" t="s">
         <v>2442</v>
       </c>
-    </row>
-    <row r="2601" spans="1:2">
+      <c r="C2600" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:3">
       <c r="A2601">
         <v>559333</v>
       </c>
       <c r="B2601" t="s">
         <v>2443</v>
       </c>
-    </row>
-    <row r="2602" spans="1:2">
+      <c r="C2601" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:3">
       <c r="A2602">
         <v>543219</v>
       </c>
       <c r="B2602" t="s">
         <v>2444</v>
       </c>
-    </row>
-    <row r="2603" spans="1:2">
+      <c r="C2602" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:3">
       <c r="A2603">
         <v>543220</v>
       </c>
       <c r="B2603" t="s">
         <v>2445</v>
       </c>
-    </row>
-    <row r="2604" spans="1:2">
+      <c r="C2603" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:3">
       <c r="A2604">
         <v>543221</v>
       </c>
       <c r="B2604" t="s">
         <v>2446</v>
       </c>
-    </row>
-    <row r="2605" spans="1:2">
+      <c r="C2604" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:3">
       <c r="A2605">
         <v>543222</v>
       </c>
       <c r="B2605" t="s">
         <v>2447</v>
       </c>
-    </row>
-    <row r="2606" spans="1:2">
+      <c r="C2605" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:3">
       <c r="A2606">
         <v>543224</v>
       </c>
       <c r="B2606" t="s">
         <v>2448</v>
       </c>
-    </row>
-    <row r="2607" spans="1:2">
+      <c r="C2606" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:3">
       <c r="A2607">
         <v>543225</v>
       </c>
       <c r="B2607" t="s">
         <v>2449</v>
       </c>
-    </row>
-    <row r="2608" spans="1:2">
+      <c r="C2607" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:3">
       <c r="A2608">
         <v>543226</v>
       </c>
       <c r="B2608" t="s">
         <v>2450</v>
       </c>
-    </row>
-    <row r="2609" spans="1:2">
+      <c r="C2608" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:3">
       <c r="A2609">
         <v>543227</v>
       </c>
       <c r="B2609" t="s">
         <v>2451</v>
       </c>
-    </row>
-    <row r="2610" spans="1:2">
+      <c r="C2609" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:3">
       <c r="A2610">
         <v>543228</v>
       </c>
       <c r="B2610" t="s">
         <v>2452</v>
       </c>
-    </row>
-    <row r="2611" spans="1:2">
+      <c r="C2610" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:3">
       <c r="A2611">
         <v>543229</v>
       </c>
       <c r="B2611" t="s">
         <v>2453</v>
       </c>
-    </row>
-    <row r="2612" spans="1:2">
+      <c r="C2611" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:3">
       <c r="A2612">
         <v>543230</v>
       </c>
       <c r="B2612" t="s">
         <v>2454</v>
       </c>
-    </row>
-    <row r="2613" spans="1:2">
+      <c r="C2612" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:3">
       <c r="A2613">
         <v>543458</v>
       </c>
       <c r="B2613" t="s">
         <v>2455</v>
       </c>
-    </row>
-    <row r="2614" spans="1:2">
+      <c r="C2613" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:3">
       <c r="A2614">
         <v>559299</v>
       </c>
       <c r="B2614" t="s">
         <v>2456</v>
       </c>
-    </row>
-    <row r="2615" spans="1:2">
+      <c r="C2614" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:3">
       <c r="A2615">
         <v>543466</v>
       </c>
       <c r="B2615" t="s">
         <v>2457</v>
       </c>
-    </row>
-    <row r="2616" spans="1:2">
+      <c r="C2615" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:3">
       <c r="A2616">
         <v>563438</v>
       </c>
       <c r="B2616" t="s">
         <v>2458</v>
       </c>
-    </row>
-    <row r="2617" spans="1:2">
+      <c r="C2616" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:3">
       <c r="A2617">
         <v>543467</v>
       </c>
       <c r="B2617" t="s">
         <v>2459</v>
       </c>
-    </row>
-    <row r="2618" spans="1:2">
+      <c r="C2617" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:3">
       <c r="A2618">
         <v>827677</v>
       </c>
       <c r="B2618" t="s">
         <v>2460</v>
       </c>
-    </row>
-    <row r="2619" spans="1:2">
+      <c r="C2618" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:3">
       <c r="A2619">
         <v>543469</v>
       </c>
       <c r="B2619" t="s">
         <v>2461</v>
       </c>
-    </row>
-    <row r="2620" spans="1:2">
+      <c r="C2619" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:3">
       <c r="A2620">
         <v>559339</v>
       </c>
       <c r="B2620" t="s">
         <v>2462</v>
       </c>
-    </row>
-    <row r="2621" spans="1:2">
+      <c r="C2620" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:3">
       <c r="A2621">
         <v>543475</v>
       </c>
       <c r="B2621" t="s">
         <v>2463</v>
       </c>
-    </row>
-    <row r="2622" spans="1:2">
+      <c r="C2621" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:3">
       <c r="A2622">
         <v>543477</v>
       </c>
       <c r="B2622" t="s">
         <v>2464</v>
       </c>
-    </row>
-    <row r="2623" spans="1:2">
+      <c r="C2622" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:3">
       <c r="A2623">
         <v>543479</v>
       </c>
       <c r="B2623" t="s">
         <v>2465</v>
       </c>
-    </row>
-    <row r="2624" spans="1:2">
+      <c r="C2623" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:3">
       <c r="A2624">
         <v>543195</v>
       </c>
       <c r="B2624" t="s">
         <v>2466</v>
       </c>
-    </row>
-    <row r="2625" spans="1:2">
+      <c r="C2624" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:3">
       <c r="A2625">
         <v>816742</v>
       </c>
       <c r="B2625" t="s">
         <v>2467</v>
       </c>
-    </row>
-    <row r="2626" spans="1:2">
+      <c r="C2625" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:3">
       <c r="A2626">
         <v>559249</v>
       </c>
       <c r="B2626" t="s">
         <v>2468</v>
       </c>
-    </row>
-    <row r="2627" spans="1:2">
+      <c r="C2626" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:3">
       <c r="A2627">
         <v>559251</v>
       </c>
       <c r="B2627" t="s">
         <v>2469</v>
       </c>
-    </row>
-    <row r="2628" spans="1:2">
+      <c r="C2627" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:3">
       <c r="A2628">
         <v>553619</v>
       </c>
       <c r="B2628" t="s">
         <v>2470</v>
       </c>
-    </row>
-    <row r="2629" spans="1:2">
+      <c r="C2628" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:3">
       <c r="A2629">
         <v>553620</v>
       </c>
       <c r="B2629" t="s">
         <v>2471</v>
       </c>
-    </row>
-    <row r="2630" spans="1:2">
+      <c r="C2629" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:3">
       <c r="A2630">
         <v>553621</v>
       </c>
       <c r="B2630" t="s">
         <v>2472</v>
       </c>
-    </row>
-    <row r="2631" spans="1:2">
+      <c r="C2630" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:3">
       <c r="A2631">
         <v>553622</v>
       </c>
       <c r="B2631" t="s">
         <v>2473</v>
       </c>
-    </row>
-    <row r="2632" spans="1:2">
+      <c r="C2631" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:3">
       <c r="A2632">
         <v>553629</v>
       </c>
       <c r="B2632" t="s">
         <v>2474</v>
       </c>
-    </row>
-    <row r="2633" spans="1:2">
+      <c r="C2632" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:3">
       <c r="A2633">
         <v>553624</v>
       </c>
       <c r="B2633" t="s">
         <v>2475</v>
       </c>
-    </row>
-    <row r="2634" spans="1:2">
+      <c r="C2633" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:3">
       <c r="A2634">
         <v>553625</v>
       </c>
       <c r="B2634" t="s">
         <v>2476</v>
       </c>
-    </row>
-    <row r="2635" spans="1:2">
+      <c r="C2634" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:3">
       <c r="A2635">
         <v>553626</v>
       </c>
       <c r="B2635" t="s">
         <v>2477</v>
       </c>
-    </row>
-    <row r="2636" spans="1:2">
+      <c r="C2635" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:3">
       <c r="A2636">
         <v>553627</v>
       </c>
       <c r="B2636" t="s">
         <v>2478</v>
       </c>
-    </row>
-    <row r="2637" spans="1:2">
+      <c r="C2636" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:3">
       <c r="A2637">
         <v>553628</v>
       </c>
       <c r="B2637" t="s">
         <v>2479</v>
       </c>
-    </row>
-    <row r="2638" spans="1:2">
+      <c r="C2637" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:3">
       <c r="A2638">
         <v>563440</v>
       </c>
       <c r="B2638" t="s">
         <v>2480</v>
       </c>
-    </row>
-    <row r="2639" spans="1:2">
+      <c r="C2638" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:3">
       <c r="A2639">
         <v>563451</v>
       </c>
       <c r="B2639" t="s">
         <v>2481</v>
       </c>
-    </row>
-    <row r="2640" spans="1:2">
+      <c r="C2639" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:3">
       <c r="A2640">
         <v>563484</v>
       </c>
       <c r="B2640" t="s">
         <v>2482</v>
       </c>
-    </row>
-    <row r="2641" spans="1:2">
+      <c r="C2640" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:3">
       <c r="A2641">
         <v>543196</v>
       </c>
       <c r="B2641" t="s">
         <v>2483</v>
       </c>
-    </row>
-    <row r="2642" spans="1:2">
+      <c r="C2641" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:3">
       <c r="A2642">
         <v>559268</v>
       </c>
       <c r="B2642" t="s">
         <v>2484</v>
       </c>
-    </row>
-    <row r="2643" spans="1:2">
+      <c r="C2642" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:3">
       <c r="A2643">
         <v>559237</v>
       </c>
       <c r="B2643" t="s">
         <v>2485</v>
       </c>
-    </row>
-    <row r="2644" spans="1:2">
+      <c r="C2643" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:3">
       <c r="A2644">
         <v>559271</v>
       </c>
       <c r="B2644" t="s">
         <v>2486</v>
       </c>
-    </row>
-    <row r="2645" spans="1:2">
+      <c r="C2644" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:3">
       <c r="A2645">
         <v>559250</v>
       </c>
       <c r="B2645" t="s">
         <v>2487</v>
       </c>
-    </row>
-    <row r="2646" spans="1:2">
+      <c r="C2645" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:3">
       <c r="A2646">
         <v>559252</v>
       </c>
       <c r="B2646" t="s">
         <v>2488</v>
       </c>
-    </row>
-    <row r="2647" spans="1:2">
+      <c r="C2646" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:3">
       <c r="A2647">
         <v>568742</v>
       </c>
       <c r="B2647" t="s">
         <v>2489</v>
       </c>
-    </row>
-    <row r="2648" spans="1:2">
+      <c r="C2647" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:3">
       <c r="A2648">
         <v>559253</v>
       </c>
       <c r="B2648" t="s">
         <v>2490</v>
       </c>
-    </row>
-    <row r="2649" spans="1:2">
+      <c r="C2648" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:3">
       <c r="A2649">
         <v>559257</v>
       </c>
       <c r="B2649" t="s">
         <v>2491</v>
       </c>
-    </row>
-    <row r="2650" spans="1:2">
+      <c r="C2649" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:3">
       <c r="A2650">
         <v>827678</v>
       </c>
       <c r="B2650" t="s">
         <v>2492</v>
       </c>
-    </row>
-    <row r="2651" spans="1:2">
+      <c r="C2650" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:3">
       <c r="A2651">
         <v>543476</v>
       </c>
       <c r="B2651" t="s">
         <v>2493</v>
       </c>
-    </row>
-    <row r="2652" spans="1:2">
+      <c r="C2651" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:3">
       <c r="A2652">
         <v>543478</v>
       </c>
       <c r="B2652" t="s">
         <v>2494</v>
       </c>
-    </row>
-    <row r="2653" spans="1:2">
+      <c r="C2652" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:3">
       <c r="A2653">
         <v>543480</v>
       </c>
       <c r="B2653" t="s">
         <v>2495</v>
       </c>
-    </row>
-    <row r="2654" spans="1:2">
+      <c r="C2653" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:3">
       <c r="A2654">
         <v>559277</v>
       </c>
       <c r="B2654" t="s">
         <v>2496</v>
       </c>
-    </row>
-    <row r="2655" spans="1:2">
+      <c r="C2654" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:3">
       <c r="A2655">
         <v>559278</v>
       </c>
       <c r="B2655" t="s">
         <v>2497</v>
       </c>
-    </row>
-    <row r="2656" spans="1:2">
+      <c r="C2655" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:3">
       <c r="A2656">
         <v>580738</v>
       </c>
       <c r="B2656" t="s">
         <v>2498</v>
       </c>
-    </row>
-    <row r="2657" spans="1:2">
+      <c r="C2656" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:3">
       <c r="A2657">
         <v>580737</v>
       </c>
       <c r="B2657" t="s">
         <v>2499</v>
       </c>
-    </row>
-    <row r="2658" spans="1:2">
+      <c r="C2657" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:3">
       <c r="A2658">
         <v>559279</v>
       </c>
       <c r="B2658" t="s">
         <v>2500</v>
       </c>
-    </row>
-    <row r="2659" spans="1:2">
+      <c r="C2658" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:3">
       <c r="A2659">
         <v>559280</v>
       </c>
       <c r="B2659" t="s">
         <v>2501</v>
       </c>
-    </row>
-    <row r="2660" spans="1:2">
+      <c r="C2659" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:3">
       <c r="A2660">
         <v>559281</v>
       </c>
       <c r="B2660" t="s">
         <v>2502</v>
       </c>
-    </row>
-    <row r="2661" spans="1:2">
+      <c r="C2660" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:3">
       <c r="A2661">
         <v>559282</v>
       </c>
       <c r="B2661" t="s">
         <v>2503</v>
       </c>
-    </row>
-    <row r="2662" spans="1:2">
+      <c r="C2661" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:3">
       <c r="A2662">
         <v>580739</v>
       </c>
       <c r="B2662" t="s">
         <v>2503</v>
       </c>
-    </row>
-    <row r="2663" spans="1:2">
+      <c r="C2662" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:3">
       <c r="A2663">
         <v>559283</v>
       </c>
       <c r="B2663" t="s">
         <v>2504</v>
       </c>
-    </row>
-    <row r="2664" spans="1:2">
+      <c r="C2663" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:3">
       <c r="A2664">
         <v>559284</v>
       </c>
       <c r="B2664" t="s">
         <v>2505</v>
       </c>
-    </row>
-    <row r="2665" spans="1:2">
+      <c r="C2664" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:3">
       <c r="A2665">
         <v>580740</v>
       </c>
       <c r="B2665" t="s">
         <v>2506</v>
       </c>
-    </row>
-    <row r="2666" spans="1:2">
+      <c r="C2665" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:3">
       <c r="A2666">
         <v>559285</v>
       </c>
       <c r="B2666" t="s">
         <v>2507</v>
       </c>
-    </row>
-    <row r="2667" spans="1:2">
+      <c r="C2666" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:3">
       <c r="A2667">
         <v>580741</v>
       </c>
       <c r="B2667" t="s">
         <v>2508</v>
       </c>
-    </row>
-    <row r="2668" spans="1:2">
+      <c r="C2667" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:3">
       <c r="A2668">
         <v>559286</v>
       </c>
       <c r="B2668" t="s">
         <v>2509</v>
       </c>
-    </row>
-    <row r="2669" spans="1:2">
+      <c r="C2668" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:3">
       <c r="A2669">
         <v>563500</v>
       </c>
       <c r="B2669" t="s">
         <v>2510</v>
       </c>
-    </row>
-    <row r="2670" spans="1:2">
+      <c r="C2669" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:3">
       <c r="A2670">
         <v>563501</v>
       </c>
       <c r="B2670" t="s">
         <v>2511</v>
       </c>
-    </row>
-    <row r="2671" spans="1:2">
+      <c r="C2670" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:3">
       <c r="A2671">
         <v>563497</v>
       </c>
       <c r="B2671" t="s">
         <v>2512</v>
       </c>
-    </row>
-    <row r="2672" spans="1:2">
+      <c r="C2671" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:3">
       <c r="A2672">
         <v>563495</v>
       </c>
       <c r="B2672" t="s">
         <v>2513</v>
       </c>
-    </row>
-    <row r="2673" spans="1:2">
+      <c r="C2672" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:3">
       <c r="A2673">
         <v>34932</v>
       </c>
       <c r="B2673" t="s">
         <v>2514</v>
       </c>
-    </row>
-    <row r="2674" spans="1:2">
+      <c r="C2673" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:3">
       <c r="A2674">
         <v>543460</v>
       </c>
       <c r="B2674" t="s">
         <v>2515</v>
       </c>
-    </row>
-    <row r="2675" spans="1:2">
+      <c r="C2674" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:3">
       <c r="A2675">
         <v>543470</v>
       </c>
       <c r="B2675" t="s">
         <v>2516</v>
       </c>
-    </row>
-    <row r="2676" spans="1:2">
+      <c r="C2675" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:3">
       <c r="A2676">
         <v>553630</v>
       </c>
       <c r="B2676" t="s">
         <v>2517</v>
       </c>
-    </row>
-    <row r="2677" spans="1:2">
+      <c r="C2676" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:3">
       <c r="A2677">
         <v>559233</v>
       </c>
       <c r="B2677" t="s">
         <v>2518</v>
       </c>
-    </row>
-    <row r="2678" spans="1:2">
+      <c r="C2677" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:3">
       <c r="A2678">
         <v>563445</v>
       </c>
       <c r="B2678" t="s">
         <v>2519</v>
       </c>
-    </row>
-    <row r="2679" spans="1:2">
+      <c r="C2678" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:3">
       <c r="A2679">
         <v>563446</v>
       </c>
       <c r="B2679" t="s">
         <v>2520</v>
       </c>
-    </row>
-    <row r="2680" spans="1:2">
+      <c r="C2679" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:3">
       <c r="A2680">
         <v>559240</v>
       </c>
       <c r="B2680" t="s">
         <v>2521</v>
       </c>
-    </row>
-    <row r="2681" spans="1:2">
+      <c r="C2680" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:3">
       <c r="A2681">
         <v>559290</v>
       </c>
       <c r="B2681" t="s">
         <v>2522</v>
       </c>
-    </row>
-    <row r="2682" spans="1:2">
+      <c r="C2681" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:3">
       <c r="A2682">
         <v>559305</v>
       </c>
       <c r="B2682" t="s">
         <v>2523</v>
       </c>
-    </row>
-    <row r="2683" spans="1:2">
+      <c r="C2682" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:3">
       <c r="A2683">
         <v>559291</v>
       </c>
       <c r="B2683" t="s">
         <v>2524</v>
       </c>
-    </row>
-    <row r="2684" spans="1:2">
+      <c r="C2683" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:3">
       <c r="A2684">
         <v>559304</v>
       </c>
       <c r="B2684" t="s">
         <v>2525</v>
       </c>
-    </row>
-    <row r="2685" spans="1:2">
+      <c r="C2684" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:3">
       <c r="A2685">
         <v>559292</v>
       </c>
       <c r="B2685" t="s">
         <v>2526</v>
       </c>
-    </row>
-    <row r="2686" spans="1:2">
+      <c r="C2685" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:3">
       <c r="A2686">
         <v>559300</v>
       </c>
       <c r="B2686" t="s">
         <v>2527</v>
       </c>
-    </row>
-    <row r="2687" spans="1:2">
+      <c r="C2686" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:3">
       <c r="A2687">
         <v>559294</v>
       </c>
       <c r="B2687" t="s">
         <v>2528</v>
       </c>
-    </row>
-    <row r="2688" spans="1:2">
+      <c r="C2687" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:3">
       <c r="A2688">
         <v>559295</v>
       </c>
       <c r="B2688" t="s">
         <v>2529</v>
       </c>
-    </row>
-    <row r="2689" spans="1:2">
+      <c r="C2688" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:3">
       <c r="A2689">
         <v>559323</v>
       </c>
       <c r="B2689" t="s">
         <v>2530</v>
       </c>
-    </row>
-    <row r="2690" spans="1:2">
+      <c r="C2689" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:3">
       <c r="A2690">
         <v>559325</v>
       </c>
       <c r="B2690" t="s">
         <v>2531</v>
       </c>
-    </row>
-    <row r="2691" spans="1:2">
+      <c r="C2690" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:3">
       <c r="A2691">
         <v>559327</v>
       </c>
       <c r="B2691" t="s">
         <v>2532</v>
       </c>
-    </row>
-    <row r="2692" spans="1:2">
+      <c r="C2691" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:3">
       <c r="A2692">
         <v>559336</v>
       </c>
       <c r="B2692" t="s">
         <v>2533</v>
       </c>
-    </row>
-    <row r="2693" spans="1:2">
+      <c r="C2692" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:3">
       <c r="A2693">
         <v>559343</v>
       </c>
       <c r="B2693" t="s">
         <v>2534</v>
       </c>
-    </row>
-    <row r="2694" spans="1:2">
+      <c r="C2693" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:3">
       <c r="A2694">
         <v>559340</v>
       </c>
       <c r="B2694" t="s">
         <v>2535</v>
       </c>
-    </row>
-    <row r="2695" spans="1:2">
+      <c r="C2694" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:3">
       <c r="A2695">
         <v>563434</v>
       </c>
       <c r="B2695" t="s">
         <v>2536</v>
       </c>
-    </row>
-    <row r="2696" spans="1:2">
+      <c r="C2695" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:3">
       <c r="A2696">
         <v>568745</v>
       </c>
       <c r="B2696" t="s">
         <v>2537</v>
       </c>
-    </row>
-    <row r="2697" spans="1:2">
+      <c r="C2696" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:3">
       <c r="A2697">
         <v>559345</v>
       </c>
       <c r="B2697" t="s">
         <v>2538</v>
       </c>
-    </row>
-    <row r="2698" spans="1:2">
+      <c r="C2697" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:3">
       <c r="A2698">
         <v>559243</v>
       </c>
       <c r="B2698" t="s">
         <v>2539</v>
       </c>
-    </row>
-    <row r="2699" spans="1:2">
+      <c r="C2698" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:3">
       <c r="A2699">
         <v>816743</v>
       </c>
       <c r="B2699" t="s">
         <v>2540</v>
       </c>
-    </row>
-    <row r="2700" spans="1:2">
+      <c r="C2699" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:3">
       <c r="A2700">
         <v>559247</v>
       </c>
       <c r="B2700" t="s">
         <v>2541</v>
       </c>
-    </row>
-    <row r="2701" spans="1:2">
+      <c r="C2700" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:3">
       <c r="A2701">
         <v>559254</v>
       </c>
       <c r="B2701" t="s">
         <v>2542</v>
       </c>
-    </row>
-    <row r="2702" spans="1:2">
+      <c r="C2701" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:3">
       <c r="A2702">
         <v>559258</v>
       </c>
       <c r="B2702" t="s">
         <v>2543</v>
       </c>
-    </row>
-    <row r="2703" spans="1:2">
+      <c r="C2702" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:3">
       <c r="A2703">
         <v>559322</v>
       </c>
       <c r="B2703" t="s">
         <v>2544</v>
       </c>
-    </row>
-    <row r="2704" spans="1:2">
+      <c r="C2703" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:3">
       <c r="A2704">
         <v>559324</v>
       </c>
       <c r="B2704" t="s">
         <v>2545</v>
       </c>
-    </row>
-    <row r="2705" spans="1:2">
+      <c r="C2704" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:3">
       <c r="A2705">
         <v>559326</v>
       </c>
       <c r="B2705" t="s">
         <v>2546</v>
       </c>
-    </row>
-    <row r="2706" spans="1:2">
+      <c r="C2705" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:3">
       <c r="A2706">
         <v>563462</v>
       </c>
       <c r="B2706" t="s">
         <v>2547</v>
       </c>
-    </row>
-    <row r="2707" spans="1:2">
+      <c r="C2706" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:3">
       <c r="A2707">
         <v>563464</v>
       </c>
       <c r="B2707" t="s">
         <v>2548</v>
       </c>
-    </row>
-    <row r="2708" spans="1:2">
+      <c r="C2707" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:3">
       <c r="A2708">
         <v>563466</v>
       </c>
       <c r="B2708" t="s">
         <v>2549</v>
       </c>
-    </row>
-    <row r="2709" spans="1:2">
+      <c r="C2708" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:3">
       <c r="A2709">
         <v>563468</v>
       </c>
       <c r="B2709" t="s">
         <v>2550</v>
       </c>
-    </row>
-    <row r="2710" spans="1:2">
+      <c r="C2709" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:3">
       <c r="A2710">
         <v>563470</v>
       </c>
       <c r="B2710" t="s">
         <v>2551</v>
       </c>
-    </row>
-    <row r="2711" spans="1:2">
+      <c r="C2710" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:3">
       <c r="A2711">
         <v>563472</v>
       </c>
       <c r="B2711" t="s">
         <v>2552</v>
       </c>
-    </row>
-    <row r="2712" spans="1:2">
+      <c r="C2711" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:3">
       <c r="A2712">
         <v>563474</v>
       </c>
       <c r="B2712" t="s">
         <v>2553</v>
       </c>
-    </row>
-    <row r="2713" spans="1:2">
+      <c r="C2712" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:3">
       <c r="A2713">
         <v>563476</v>
       </c>
       <c r="B2713" t="s">
         <v>2554</v>
       </c>
-    </row>
-    <row r="2714" spans="1:2">
+      <c r="C2713" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:3">
       <c r="A2714">
         <v>568724</v>
       </c>
       <c r="B2714" t="s">
         <v>2555</v>
       </c>
-    </row>
-    <row r="2715" spans="1:2">
+      <c r="C2714" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:3">
       <c r="A2715">
         <v>563458</v>
       </c>
       <c r="B2715" t="s">
         <v>2556</v>
       </c>
-    </row>
-    <row r="2716" spans="1:2">
+      <c r="C2715" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:3">
       <c r="A2716">
         <v>563485</v>
       </c>
       <c r="B2716" t="s">
         <v>2557</v>
       </c>
-    </row>
-    <row r="2717" spans="1:2">
+      <c r="C2716" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:3">
       <c r="A2717">
         <v>559331</v>
       </c>
       <c r="B2717" t="s">
         <v>2558</v>
       </c>
-    </row>
-    <row r="2718" spans="1:2">
+      <c r="C2717" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:3">
       <c r="A2718">
         <v>559335</v>
       </c>
       <c r="B2718" t="s">
         <v>2559</v>
       </c>
-    </row>
-    <row r="2719" spans="1:2">
+      <c r="C2718" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:3">
       <c r="A2719">
         <v>559297</v>
       </c>
       <c r="B2719" t="s">
         <v>2560</v>
       </c>
-    </row>
-    <row r="2720" spans="1:2">
+      <c r="C2719" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:3">
       <c r="A2720">
         <v>559303</v>
       </c>
       <c r="B2720" t="s">
         <v>2561</v>
       </c>
-    </row>
-    <row r="2721" spans="1:2">
+      <c r="C2720" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:3">
       <c r="A2721">
         <v>563457</v>
       </c>
       <c r="B2721" t="s">
         <v>2562</v>
       </c>
-    </row>
-    <row r="2722" spans="1:2">
+      <c r="C2721" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:3">
       <c r="A2722">
         <v>563455</v>
       </c>
       <c r="B2722" t="s">
         <v>2563</v>
       </c>
-    </row>
-    <row r="2723" spans="1:2">
+      <c r="C2722" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:3">
       <c r="A2723">
         <v>543459</v>
       </c>
       <c r="B2723" t="s">
         <v>2564</v>
       </c>
-    </row>
-    <row r="2724" spans="1:2">
+      <c r="C2723" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:3">
       <c r="A2724">
         <v>568719</v>
       </c>
       <c r="B2724" t="s">
         <v>2565</v>
       </c>
-    </row>
-    <row r="2725" spans="1:2">
+      <c r="C2724" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:3">
       <c r="A2725">
         <v>559338</v>
       </c>
       <c r="B2725" t="s">
         <v>2566</v>
       </c>
-    </row>
-    <row r="2726" spans="1:2">
+      <c r="C2725" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:3">
       <c r="A2726">
         <v>559337</v>
       </c>
       <c r="B2726" t="s">
         <v>2567</v>
       </c>
-    </row>
-    <row r="2727" spans="1:2">
+      <c r="C2726" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:3">
       <c r="A2727">
         <v>559344</v>
       </c>
       <c r="B2727" t="s">
         <v>2568</v>
       </c>
-    </row>
-    <row r="2728" spans="1:2">
+      <c r="C2727" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:3">
       <c r="A2728">
         <v>559332</v>
       </c>
       <c r="B2728" t="s">
         <v>2569</v>
       </c>
-    </row>
-    <row r="2729" spans="1:2">
+      <c r="C2728" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:3">
       <c r="A2729">
         <v>563452</v>
       </c>
       <c r="B2729" t="s">
         <v>2570</v>
       </c>
-    </row>
-    <row r="2730" spans="1:2">
+      <c r="C2729" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:3">
       <c r="A2730">
         <v>559298</v>
       </c>
       <c r="B2730" t="s">
         <v>2571</v>
       </c>
-    </row>
-    <row r="2731" spans="1:2">
+      <c r="C2730" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:3">
       <c r="A2731">
         <v>563454</v>
       </c>
       <c r="B2731" t="s">
         <v>2572</v>
       </c>
-    </row>
-    <row r="2732" spans="1:2">
+      <c r="C2731" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:3">
       <c r="A2732">
         <v>563456</v>
       </c>
       <c r="B2732" t="s">
         <v>2573</v>
       </c>
-    </row>
-    <row r="2733" spans="1:2">
+      <c r="C2732" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:3">
       <c r="A2733">
         <v>568749</v>
       </c>
       <c r="B2733" t="s">
         <v>2574</v>
       </c>
-    </row>
-    <row r="2734" spans="1:2">
+      <c r="C2733" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:3">
       <c r="A2734">
         <v>543194</v>
       </c>
       <c r="B2734" t="s">
         <v>2575</v>
       </c>
-    </row>
-    <row r="2735" spans="1:2">
+      <c r="C2734" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:3">
       <c r="A2735">
         <v>559248</v>
       </c>
       <c r="B2735" t="s">
         <v>2576</v>
       </c>
-    </row>
-    <row r="2736" spans="1:2">
+      <c r="C2735" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:3">
       <c r="A2736">
         <v>559256</v>
       </c>
       <c r="B2736" t="s">
         <v>2577</v>
       </c>
-    </row>
-    <row r="2737" spans="1:2">
+      <c r="C2736" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:3">
       <c r="A2737">
         <v>559276</v>
       </c>
       <c r="B2737" t="s">
         <v>2578</v>
       </c>
-    </row>
-    <row r="2738" spans="1:2">
+      <c r="C2737" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:3">
       <c r="A2738">
         <v>568726</v>
       </c>
       <c r="B2738" t="s">
         <v>2579</v>
       </c>
-    </row>
-    <row r="2739" spans="1:2">
+      <c r="C2738" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:3">
       <c r="A2739">
         <v>568729</v>
       </c>
       <c r="B2739" t="s">
         <v>2580</v>
       </c>
-    </row>
-    <row r="2740" spans="1:2">
+      <c r="C2739" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:3">
       <c r="A2740">
         <v>563460</v>
       </c>
       <c r="B2740" t="s">
         <v>2581</v>
       </c>
-    </row>
-    <row r="2741" spans="1:2">
+      <c r="C2740" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:3">
       <c r="A2741">
         <v>559287</v>
       </c>
       <c r="B2741" t="s">
         <v>2582</v>
       </c>
-    </row>
-    <row r="2742" spans="1:2">
+      <c r="C2741" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:3">
       <c r="A2742">
         <v>563489</v>
       </c>
       <c r="B2742" t="s">
         <v>2583</v>
       </c>
-    </row>
-    <row r="2743" spans="1:2">
+      <c r="C2742" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:3">
       <c r="A2743">
         <v>563494</v>
       </c>
       <c r="B2743" t="s">
         <v>2584</v>
       </c>
-    </row>
-    <row r="2744" spans="1:2">
+      <c r="C2743" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:3">
       <c r="A2744">
         <v>563493</v>
       </c>
       <c r="B2744" t="s">
         <v>2585</v>
       </c>
-    </row>
-    <row r="2745" spans="1:2">
+      <c r="C2744" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:3">
       <c r="A2745">
         <v>563498</v>
       </c>
       <c r="B2745" t="s">
         <v>2586</v>
       </c>
-    </row>
-    <row r="2746" spans="1:2">
+      <c r="C2745" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:3">
       <c r="A2746">
         <v>563490</v>
       </c>
       <c r="B2746" t="s">
         <v>2587</v>
       </c>
-    </row>
-    <row r="2747" spans="1:2">
+      <c r="C2746" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:3">
       <c r="A2747">
         <v>563499</v>
       </c>
       <c r="B2747" t="s">
         <v>2588</v>
       </c>
-    </row>
-    <row r="2748" spans="1:2">
+      <c r="C2747" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:3">
       <c r="A2748">
         <v>563502</v>
       </c>
       <c r="B2748" t="s">
         <v>2589</v>
       </c>
-    </row>
-    <row r="2749" spans="1:2">
+      <c r="C2748" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:3">
       <c r="A2749">
         <v>559245</v>
       </c>
       <c r="B2749" t="s">
         <v>2590</v>
       </c>
-    </row>
-    <row r="2750" spans="1:2">
+      <c r="C2749" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:3">
       <c r="A2750">
         <v>559267</v>
       </c>
       <c r="B2750" t="s">
         <v>2591</v>
       </c>
-    </row>
-    <row r="2751" spans="1:2">
+      <c r="C2750" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:3">
       <c r="A2751">
         <v>725503</v>
       </c>
       <c r="B2751" t="s">
         <v>2592</v>
       </c>
-    </row>
-    <row r="2752" spans="1:2">
+      <c r="C2751" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:3">
       <c r="A2752">
         <v>559274</v>
       </c>
       <c r="B2752" t="s">
         <v>2593</v>
       </c>
-    </row>
-    <row r="2753" spans="1:2">
+      <c r="C2752" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:3">
       <c r="A2753">
         <v>559236</v>
       </c>
       <c r="B2753" t="s">
         <v>2594</v>
       </c>
-    </row>
-    <row r="2754" spans="1:2">
+      <c r="C2753" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:3">
       <c r="A2754">
         <v>568723</v>
       </c>
       <c r="B2754" t="s">
         <v>2595</v>
       </c>
-    </row>
-    <row r="2755" spans="1:2">
+      <c r="C2754" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:3">
       <c r="A2755">
         <v>559270</v>
       </c>
       <c r="B2755" t="s">
         <v>2596</v>
       </c>
-    </row>
-    <row r="2756" spans="1:2">
+      <c r="C2755" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:3">
       <c r="A2756">
         <v>568750</v>
       </c>
       <c r="B2756" t="s">
         <v>2597</v>
       </c>
-    </row>
-    <row r="2757" spans="1:2">
+      <c r="C2756" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:3">
       <c r="A2757">
         <v>543474</v>
       </c>
       <c r="B2757" t="s">
         <v>2598</v>
       </c>
-    </row>
-    <row r="2758" spans="1:2">
+      <c r="C2757" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:3">
       <c r="A2758">
         <v>559244</v>
       </c>
       <c r="B2758" t="s">
         <v>2599</v>
       </c>
-    </row>
-    <row r="2759" spans="1:2">
+      <c r="C2758" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:3">
       <c r="A2759">
         <v>559266</v>
       </c>
       <c r="B2759" t="s">
         <v>2600</v>
       </c>
-    </row>
-    <row r="2760" spans="1:2">
+      <c r="C2759" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:3">
       <c r="A2760">
         <v>725502</v>
       </c>
       <c r="B2760" t="s">
         <v>2601</v>
       </c>
-    </row>
-    <row r="2761" spans="1:2">
+      <c r="C2760" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:3">
       <c r="A2761">
         <v>559273</v>
       </c>
       <c r="B2761" t="s">
         <v>2602</v>
       </c>
-    </row>
-    <row r="2762" spans="1:2">
+      <c r="C2761" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:3">
       <c r="A2762">
         <v>568722</v>
       </c>
       <c r="B2762" t="s">
         <v>2603</v>
       </c>
-    </row>
-    <row r="2763" spans="1:2">
+      <c r="C2762" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:3">
       <c r="A2763">
         <v>559269</v>
       </c>
       <c r="B2763" t="s">
         <v>2604</v>
       </c>
-    </row>
-    <row r="2764" spans="1:2">
+      <c r="C2763" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:3">
       <c r="A2764">
         <v>563437</v>
       </c>
       <c r="B2764" t="s">
         <v>2605</v>
       </c>
-    </row>
-    <row r="2765" spans="1:2">
+      <c r="C2764" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:3">
       <c r="A2765">
         <v>568738</v>
       </c>
       <c r="B2765" t="s">
         <v>2606</v>
       </c>
-    </row>
-    <row r="2766" spans="1:2">
+      <c r="C2765" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:3">
       <c r="A2766">
         <v>568720</v>
       </c>
       <c r="B2766" t="s">
         <v>2607</v>
       </c>
-    </row>
-    <row r="2767" spans="1:2">
+      <c r="C2766" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:3">
       <c r="A2767">
         <v>568751</v>
       </c>
       <c r="B2767" t="s">
         <v>2608</v>
       </c>
-    </row>
-    <row r="2768" spans="1:2">
+      <c r="C2767" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:3">
       <c r="A2768">
         <v>563449</v>
       </c>
       <c r="B2768" t="s">
         <v>2609</v>
       </c>
-    </row>
-    <row r="2769" spans="1:2">
+      <c r="C2768" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:3">
       <c r="A2769">
         <v>563448</v>
       </c>
       <c r="B2769" t="s">
         <v>2610</v>
       </c>
-    </row>
-    <row r="2770" spans="1:2">
+      <c r="C2769" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:3">
       <c r="A2770">
         <v>563450</v>
       </c>
       <c r="B2770" t="s">
         <v>2611</v>
       </c>
-    </row>
-    <row r="2771" spans="1:2">
+      <c r="C2770" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:3">
       <c r="A2771">
         <v>563447</v>
       </c>
       <c r="B2771" t="s">
         <v>2612</v>
       </c>
-    </row>
-    <row r="2772" spans="1:2">
+      <c r="C2771" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:3">
       <c r="A2772">
         <v>835451</v>
       </c>
       <c r="B2772" t="s">
         <v>2613</v>
       </c>
-    </row>
-    <row r="2773" spans="1:2">
+      <c r="C2772" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:3">
       <c r="A2773">
         <v>543461</v>
       </c>
       <c r="B2773" t="s">
         <v>2614</v>
       </c>
-    </row>
-    <row r="2774" spans="1:2">
+      <c r="C2773" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:3">
       <c r="A2774">
         <v>543464</v>
       </c>
       <c r="B2774" t="s">
         <v>2615</v>
       </c>
-    </row>
-    <row r="2775" spans="1:2">
+      <c r="C2774" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:3">
       <c r="A2775">
         <v>559288</v>
       </c>
       <c r="B2775" t="s">
         <v>2616</v>
       </c>
-    </row>
-    <row r="2776" spans="1:2">
+      <c r="C2775" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:3">
       <c r="A2776">
         <v>563453</v>
       </c>
       <c r="B2776" t="s">
         <v>2617</v>
       </c>
-    </row>
-    <row r="2777" spans="1:2">
+      <c r="C2776" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:3">
       <c r="A2777">
         <v>563483</v>
       </c>
       <c r="B2777" t="s">
         <v>2618</v>
       </c>
-    </row>
-    <row r="2778" spans="1:2">
+      <c r="C2777" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:3">
       <c r="A2778">
         <v>568736</v>
       </c>
       <c r="B2778" t="s">
         <v>2619</v>
       </c>
-    </row>
-    <row r="2779" spans="1:2">
+      <c r="C2778" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:3">
       <c r="A2779">
         <v>559328</v>
       </c>
       <c r="B2779" t="s">
         <v>2620</v>
       </c>
-    </row>
-    <row r="2780" spans="1:2">
+      <c r="C2779" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:3">
       <c r="A2780">
         <v>568741</v>
       </c>
       <c r="B2780" t="s">
         <v>2621</v>
       </c>
-    </row>
-    <row r="2781" spans="1:2">
+      <c r="C2780" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:3">
       <c r="A2781">
         <v>568735</v>
       </c>
       <c r="B2781" t="s">
         <v>2622</v>
       </c>
-    </row>
-    <row r="2782" spans="1:2">
+      <c r="C2781" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:3">
       <c r="A2782">
         <v>568740</v>
       </c>
       <c r="B2782" t="s">
         <v>2623</v>
       </c>
-    </row>
-    <row r="2783" spans="1:2">
+      <c r="C2782" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:3">
       <c r="A2783">
         <v>563461</v>
       </c>
       <c r="B2783" t="s">
         <v>2624</v>
       </c>
-    </row>
-    <row r="2784" spans="1:2">
+      <c r="C2783" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:3">
       <c r="A2784">
         <v>563463</v>
       </c>
       <c r="B2784" t="s">
         <v>2625</v>
       </c>
-    </row>
-    <row r="2785" spans="1:2">
+      <c r="C2784" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:3">
       <c r="A2785">
         <v>563465</v>
       </c>
       <c r="B2785" t="s">
         <v>2626</v>
       </c>
-    </row>
-    <row r="2786" spans="1:2">
+      <c r="C2785" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:3">
       <c r="A2786">
         <v>563467</v>
       </c>
       <c r="B2786" t="s">
         <v>2627</v>
       </c>
-    </row>
-    <row r="2787" spans="1:2">
+      <c r="C2786" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:3">
       <c r="A2787">
         <v>563469</v>
       </c>
       <c r="B2787" t="s">
         <v>2628</v>
       </c>
-    </row>
-    <row r="2788" spans="1:2">
+      <c r="C2787" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:3">
       <c r="A2788">
         <v>563471</v>
       </c>
       <c r="B2788" t="s">
         <v>2629</v>
       </c>
-    </row>
-    <row r="2789" spans="1:2">
+      <c r="C2788" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:3">
       <c r="A2789">
         <v>563473</v>
       </c>
       <c r="B2789" t="s">
         <v>2630</v>
       </c>
-    </row>
-    <row r="2790" spans="1:2">
+      <c r="C2789" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:3">
       <c r="A2790">
         <v>563475</v>
       </c>
       <c r="B2790" t="s">
         <v>2631</v>
       </c>
-    </row>
-    <row r="2791" spans="1:2">
+      <c r="C2790" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:3">
       <c r="A2791">
         <v>196635</v>
       </c>
       <c r="B2791" t="s">
         <v>2632</v>
       </c>
-    </row>
-    <row r="2792" spans="1:2">
+      <c r="C2791" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:3">
       <c r="A2792">
         <v>568748</v>
       </c>
       <c r="B2792" t="s">
         <v>2633</v>
       </c>
-    </row>
-    <row r="2793" spans="1:2">
+      <c r="C2792" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:3">
       <c r="A2793">
         <v>559302</v>
       </c>
       <c r="B2793" t="s">
         <v>2634</v>
       </c>
-    </row>
-    <row r="2794" spans="1:2">
+      <c r="C2793" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:3">
       <c r="A2794">
         <v>559301</v>
       </c>
       <c r="B2794" t="s">
         <v>2635</v>
       </c>
-    </row>
-    <row r="2795" spans="1:2">
+      <c r="C2794" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:3">
       <c r="A2795">
         <v>543481</v>
       </c>
       <c r="B2795" t="s">
         <v>2636</v>
       </c>
-    </row>
-    <row r="2796" spans="1:2">
+      <c r="C2795" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:3">
       <c r="A2796">
         <v>543463</v>
       </c>
       <c r="B2796" t="s">
         <v>2637</v>
       </c>
-    </row>
-    <row r="2797" spans="1:2">
+      <c r="C2796" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:3">
       <c r="A2797">
         <v>559235</v>
       </c>
       <c r="B2797" t="s">
         <v>2638</v>
       </c>
-    </row>
-    <row r="2798" spans="1:2">
+      <c r="C2797" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:3">
       <c r="A2798">
         <v>543468</v>
       </c>
       <c r="B2798" t="s">
         <v>2639</v>
       </c>
-    </row>
-    <row r="2799" spans="1:2">
+      <c r="C2798" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:3">
       <c r="A2799">
         <v>563433</v>
       </c>
       <c r="B2799" t="s">
         <v>2640</v>
       </c>
-    </row>
-    <row r="2800" spans="1:2">
+      <c r="C2799" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:3">
       <c r="A2800">
         <v>563486</v>
       </c>
       <c r="B2800" t="s">
         <v>2641</v>
       </c>
-    </row>
-    <row r="2801" spans="1:2">
+      <c r="C2800" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:3">
       <c r="A2801">
         <v>563492</v>
       </c>
       <c r="B2801" t="s">
         <v>2642</v>
       </c>
-    </row>
-    <row r="2802" spans="1:2">
+      <c r="C2801" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:3">
       <c r="A2802">
         <v>563488</v>
       </c>
       <c r="B2802" t="s">
         <v>2643</v>
       </c>
-    </row>
-    <row r="2803" spans="1:2">
+      <c r="C2802" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:3">
       <c r="A2803">
         <v>563496</v>
       </c>
       <c r="B2803" t="s">
         <v>2644</v>
       </c>
-    </row>
-    <row r="2804" spans="1:2">
+      <c r="C2803" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2804" spans="1:3">
       <c r="A2804">
         <v>568721</v>
       </c>
       <c r="B2804" t="s">
         <v>2645</v>
       </c>
-    </row>
-    <row r="2805" spans="1:2">
+      <c r="C2804" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2805" spans="1:3">
       <c r="A2805">
         <v>559334</v>
       </c>
       <c r="B2805" t="s">
         <v>2646</v>
       </c>
-    </row>
-    <row r="2806" spans="1:2">
+      <c r="C2805" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2806" spans="1:3">
       <c r="A2806">
         <v>543465</v>
       </c>
       <c r="B2806" t="s">
         <v>2647</v>
       </c>
-    </row>
-    <row r="2807" spans="1:2">
+      <c r="C2806" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2807" spans="1:3">
       <c r="A2807">
         <v>563491</v>
       </c>
       <c r="B2807" t="s">
         <v>2648</v>
       </c>
-    </row>
-    <row r="2808" spans="1:2">
+      <c r="C2807" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2808" spans="1:3">
       <c r="A2808">
         <v>563435</v>
       </c>
       <c r="B2808" t="s">
         <v>2649</v>
       </c>
-    </row>
-    <row r="2809" spans="1:2">
+      <c r="C2808" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2809" spans="1:3">
       <c r="A2809">
         <v>568727</v>
       </c>
       <c r="B2809" t="s">
         <v>2650</v>
       </c>
-    </row>
-    <row r="2810" spans="1:2">
+      <c r="C2809" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2810" spans="1:3">
       <c r="A2810">
         <v>563436</v>
       </c>
       <c r="B2810" t="s">
         <v>2651</v>
       </c>
-    </row>
-    <row r="2811" spans="1:2">
+      <c r="C2810" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2811" spans="1:3">
       <c r="A2811">
         <v>827680</v>
       </c>
       <c r="B2811" t="s">
         <v>2652</v>
       </c>
-    </row>
-    <row r="2812" spans="1:2">
+      <c r="C2811" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2812" spans="1:3">
       <c r="A2812">
         <v>88793</v>
       </c>
       <c r="B2812" t="s">
         <v>2653</v>
       </c>
-    </row>
-    <row r="2813" spans="1:2">
+      <c r="C2812" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2813" spans="1:3">
       <c r="A2813">
         <v>88794</v>
       </c>
       <c r="B2813" t="s">
         <v>2654</v>
       </c>
-    </row>
-    <row r="2814" spans="1:2">
+      <c r="C2813" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2814" spans="1:3">
       <c r="A2814">
         <v>88792</v>
       </c>
       <c r="B2814" t="s">
         <v>2655</v>
       </c>
-    </row>
-    <row r="2815" spans="1:2">
+      <c r="C2814" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2815" spans="1:3">
       <c r="A2815">
         <v>88791</v>
       </c>
       <c r="B2815" t="s">
         <v>2656</v>
       </c>
-    </row>
-    <row r="2816" spans="1:2">
+      <c r="C2815" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2816" spans="1:3">
       <c r="A2816">
         <v>88796</v>
       </c>
       <c r="B2816" t="s">
         <v>2657</v>
       </c>
-    </row>
-    <row r="2817" spans="1:2">
+      <c r="C2816" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2817" spans="1:3">
       <c r="A2817">
         <v>88784</v>
       </c>
       <c r="B2817" t="s">
         <v>2658</v>
       </c>
-    </row>
-    <row r="2818" spans="1:2">
+      <c r="C2817" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2818" spans="1:3">
       <c r="A2818">
         <v>568734</v>
       </c>
       <c r="B2818" t="s">
         <v>2659</v>
       </c>
-    </row>
-    <row r="2819" spans="1:2">
+      <c r="C2818" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2819" spans="1:3">
       <c r="A2819">
         <v>88787</v>
       </c>
       <c r="B2819" t="s">
         <v>2660</v>
       </c>
-    </row>
-    <row r="2820" spans="1:2">
+      <c r="C2819" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2820" spans="1:3">
       <c r="A2820">
         <v>596239</v>
       </c>
       <c r="B2820" t="s">
         <v>2661</v>
       </c>
-    </row>
-    <row r="2821" spans="1:2">
+      <c r="C2820" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2821" spans="1:3">
       <c r="A2821">
         <v>88789</v>
       </c>
       <c r="B2821" t="s">
         <v>2662</v>
       </c>
-    </row>
-    <row r="2822" spans="1:2">
+      <c r="C2821" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2822" spans="1:3">
       <c r="A2822">
         <v>88783</v>
       </c>
       <c r="B2822" t="s">
         <v>2663</v>
       </c>
-    </row>
-    <row r="2823" spans="1:2">
+      <c r="C2822" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2823" spans="1:3">
       <c r="A2823">
         <v>568730</v>
       </c>
       <c r="B2823" t="s">
         <v>2664</v>
       </c>
-    </row>
-    <row r="2824" spans="1:2">
+      <c r="C2823" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2824" spans="1:3">
       <c r="A2824">
         <v>568731</v>
       </c>
       <c r="B2824" t="s">
         <v>2665</v>
       </c>
-    </row>
-    <row r="2825" spans="1:2">
+      <c r="C2824" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2825" spans="1:3">
       <c r="A2825">
         <v>568732</v>
       </c>
       <c r="B2825" t="s">
         <v>2666</v>
       </c>
-    </row>
-    <row r="2826" spans="1:2">
+      <c r="C2825" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2826" spans="1:3">
       <c r="A2826">
         <v>88790</v>
       </c>
       <c r="B2826" t="s">
         <v>2667</v>
       </c>
-    </row>
-    <row r="2827" spans="1:2">
+      <c r="C2826" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:3">
       <c r="A2827">
         <v>88797</v>
       </c>
       <c r="B2827" t="s">
         <v>2668</v>
       </c>
-    </row>
-    <row r="2828" spans="1:2">
+      <c r="C2827" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:3">
       <c r="A2828">
         <v>88786</v>
       </c>
       <c r="B2828" t="s">
         <v>2669</v>
       </c>
-    </row>
-    <row r="2829" spans="1:2">
+      <c r="C2828" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2829" spans="1:3">
       <c r="A2829">
         <v>568733</v>
       </c>
       <c r="B2829" t="s">
         <v>2670</v>
       </c>
-    </row>
-    <row r="2830" spans="1:2">
+      <c r="C2829" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2830" spans="1:3">
       <c r="A2830">
         <v>88788</v>
       </c>
       <c r="B2830" t="s">
         <v>2671</v>
       </c>
-    </row>
-    <row r="2831" spans="1:2">
+      <c r="C2830" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2831" spans="1:3">
       <c r="A2831">
         <v>88785</v>
       </c>
       <c r="B2831" t="s">
         <v>2672</v>
       </c>
-    </row>
-    <row r="2832" spans="1:2">
+      <c r="C2831" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2832" spans="1:3">
       <c r="A2832">
         <v>88795</v>
       </c>
       <c r="B2832" t="s">
         <v>2673</v>
       </c>
-    </row>
-    <row r="2833" spans="1:2">
+      <c r="C2832" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2833" spans="1:3">
       <c r="A2833">
         <v>816744</v>
       </c>
       <c r="B2833" t="s">
         <v>2674</v>
       </c>
-    </row>
-    <row r="2834" spans="1:2">
+      <c r="C2833" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2834" spans="1:3">
       <c r="A2834">
         <v>559246</v>
       </c>
       <c r="B2834" t="s">
         <v>2675</v>
       </c>
-    </row>
-    <row r="2835" spans="1:2">
+      <c r="C2834" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2835" spans="1:3">
       <c r="A2835">
         <v>559275</v>
       </c>
       <c r="B2835" t="s">
         <v>2676</v>
       </c>
-    </row>
-    <row r="2836" spans="1:2">
+      <c r="C2835" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2836" spans="1:3">
       <c r="A2836">
         <v>559255</v>
       </c>
       <c r="B2836" t="s">
         <v>2677</v>
       </c>
-    </row>
-    <row r="2837" spans="1:2">
+      <c r="C2836" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2837" spans="1:3">
       <c r="A2837">
         <v>568725</v>
       </c>
       <c r="B2837" t="s">
         <v>2678</v>
       </c>
-    </row>
-    <row r="2838" spans="1:2">
+      <c r="C2837" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2838" spans="1:3">
       <c r="A2838">
         <v>568728</v>
       </c>
       <c r="B2838" t="s">
         <v>2679</v>
       </c>
-    </row>
-    <row r="2839" spans="1:2">
+      <c r="C2838" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2839" spans="1:3">
       <c r="A2839">
         <v>563459</v>
       </c>
       <c r="B2839" t="s">
         <v>2680</v>
       </c>
-    </row>
-    <row r="2840" spans="1:2">
+      <c r="C2839" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2840" spans="1:3">
       <c r="A2840">
         <v>559272</v>
       </c>
       <c r="B2840" t="s">
         <v>2681</v>
       </c>
-    </row>
-    <row r="2841" spans="1:2">
+      <c r="C2840" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2841" spans="1:3">
       <c r="A2841">
         <v>568737</v>
       </c>
       <c r="B2841" t="s">
         <v>2682</v>
       </c>
-    </row>
-    <row r="2842" spans="1:2">
+      <c r="C2841" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2842" spans="1:3">
       <c r="A2842">
         <v>559241</v>
       </c>
       <c r="B2842" t="s">
         <v>2683</v>
       </c>
-    </row>
-    <row r="2843" spans="1:2">
+      <c r="C2842" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2843" spans="1:3">
       <c r="A2843">
         <v>563439</v>
       </c>
       <c r="B2843" t="s">
         <v>2684</v>
       </c>
-    </row>
-    <row r="2844" spans="1:2">
+      <c r="C2843" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2844" spans="1:3">
       <c r="A2844">
         <v>559242</v>
       </c>
       <c r="B2844" t="s">
         <v>2685</v>
       </c>
-    </row>
-    <row r="2845" spans="1:2">
+      <c r="C2844" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2845" spans="1:3">
       <c r="A2845">
         <v>559329</v>
       </c>
       <c r="B2845" t="s">
         <v>2686</v>
       </c>
-    </row>
-    <row r="2846" spans="1:2">
+      <c r="C2845" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2846" spans="1:3">
       <c r="A2846">
         <v>559330</v>
       </c>
       <c r="B2846" t="s">
         <v>2687</v>
       </c>
-    </row>
-    <row r="2847" spans="1:2">
+      <c r="C2846" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2847" spans="1:3">
       <c r="A2847">
         <v>568739</v>
       </c>
       <c r="B2847" t="s">
         <v>2688</v>
       </c>
-    </row>
-    <row r="2848" spans="1:2">
+      <c r="C2847" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2848" spans="1:3">
       <c r="A2848">
         <v>559239</v>
       </c>
       <c r="B2848" t="s">
         <v>2689</v>
+      </c>
+      <c r="C2848" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2849" spans="1:3">
@@ -40884,6 +41768,9 @@
       <c r="B2849" t="s">
         <v>2690</v>
       </c>
+      <c r="C2849" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2850" spans="1:3">
       <c r="A2850">
@@ -40892,6 +41779,9 @@
       <c r="B2850" t="s">
         <v>2691</v>
       </c>
+      <c r="C2850" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2851" spans="1:3">
       <c r="A2851">
@@ -40900,6 +41790,9 @@
       <c r="B2851" t="s">
         <v>2692</v>
       </c>
+      <c r="C2851" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2852" spans="1:3">
       <c r="A2852">
@@ -40908,6 +41801,9 @@
       <c r="B2852" t="s">
         <v>2693</v>
       </c>
+      <c r="C2852" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2853" spans="1:3">
       <c r="A2853">
@@ -40916,6 +41812,9 @@
       <c r="B2853" t="s">
         <v>2694</v>
       </c>
+      <c r="C2853" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2854" spans="1:3">
       <c r="A2854">
@@ -40924,6 +41823,9 @@
       <c r="B2854" t="s">
         <v>2695</v>
       </c>
+      <c r="C2854" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2855" spans="1:3">
       <c r="A2855">
@@ -40932,6 +41834,9 @@
       <c r="B2855" t="s">
         <v>2696</v>
       </c>
+      <c r="C2855" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2856" spans="1:3">
       <c r="A2856">
@@ -40940,6 +41845,9 @@
       <c r="B2856" t="s">
         <v>2697</v>
       </c>
+      <c r="C2856" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2857" spans="1:3">
       <c r="A2857">
@@ -40948,6 +41856,9 @@
       <c r="B2857" t="s">
         <v>2698</v>
       </c>
+      <c r="C2857" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2858" spans="1:3">
       <c r="A2858">
@@ -40956,6 +41867,9 @@
       <c r="B2858" t="s">
         <v>2699</v>
       </c>
+      <c r="C2858" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2859" spans="1:3">
       <c r="A2859">
@@ -40964,6 +41878,9 @@
       <c r="B2859" t="s">
         <v>2700</v>
       </c>
+      <c r="C2859" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2860" spans="1:3">
       <c r="A2860">
@@ -40971,6 +41888,9 @@
       </c>
       <c r="B2860" t="s">
         <v>2701</v>
+      </c>
+      <c r="C2860" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2861" spans="1:3">

</xml_diff>